<commit_message>
streamlining good moral process
</commit_message>
<xml_diff>
--- a/myapp/cert_templates/good-moral-form.xlsx
+++ b/myapp/cert_templates/good-moral-form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\thesis_osa\myproject\myapp\cert_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA56FF0F-FF67-45DA-B6BB-7EB8E61AF2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB7673C-5E1C-413E-8F9C-1C4F259FB370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="student_name">inputs!$B$2</definedName>
     <definedName name="years_of_stay">inputs!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -50,6 +50,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
@@ -62,25 +84,13 @@
     <t>student_name</t>
   </si>
   <si>
-    <t>Lord Jaisson C. Riberal</t>
-  </si>
-  <si>
     <t>program</t>
-  </si>
-  <si>
-    <t>Bachelor of Engineering Technology Major in Computer Engineering Technology</t>
   </si>
   <si>
     <t>sex</t>
   </si>
   <si>
-    <t>female</t>
-  </si>
-  <si>
     <t>status</t>
-  </si>
-  <si>
-    <t>current student</t>
   </si>
   <si>
     <t>years_of_stay</t>
@@ -95,13 +105,7 @@
     <t>purpose</t>
   </si>
   <si>
-    <t>Scholarship</t>
-  </si>
-  <si>
     <t>purpose_other</t>
-  </si>
-  <si>
-    <t>DOST</t>
   </si>
   <si>
     <t>osahead</t>
@@ -162,6 +166,24 @@
   </si>
   <si>
     <t xml:space="preserve">   PC-F-OQA-DCG-14 Ø3 (03.28.25)</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>Former Student</t>
+  </si>
+  <si>
+    <t>2015-2016</t>
+  </si>
+  <si>
+    <t>Civil Engineering Technology</t>
+  </si>
+  <si>
+    <t>continuing education</t>
+  </si>
+  <si>
+    <t>CLIFF JASON D. DEYPALUBOS</t>
   </si>
 </sst>
 </file>
@@ -385,6 +407,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -399,32 +445,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1312,7 +1334,7 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{FAA26D3D-D897-4be2-8F04-BA451C77F1D7}">
-            <ma14:placeholderFlag xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" xmlns:cx3="http://schemas.microsoft.com/office/drawing/2016/5/9/chartex" xmlns:cx4="http://schemas.microsoft.com/office/drawing/2016/5/10/chartex" xmlns:cx5="http://schemas.microsoft.com/office/drawing/2016/5/11/chartex" xmlns:cx6="http://schemas.microsoft.com/office/drawing/2016/5/12/chartex" xmlns:cx7="http://schemas.microsoft.com/office/drawing/2016/5/13/chartex" xmlns:cx8="http://schemas.microsoft.com/office/drawing/2016/5/14/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" xmlns:oel="http://schemas.microsoft.com/office/2019/extlst" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:w16cex="http://schemas.microsoft.com/office/word/2018/wordml/cex" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:w16="http://schemas.microsoft.com/office/word/2018/wordml" xmlns:w16du="http://schemas.microsoft.com/office/word/2023/wordml/word16du" xmlns:w16sdtdh="http://schemas.microsoft.com/office/word/2020/wordml/sdtdatahash" xmlns:w16sdtfl="http://schemas.microsoft.com/office/word/2024/wordml/sdtformatlock" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns="" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:arto="http://schemas.microsoft.com/office/word/2006/arto" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas"/>
+            <ma14:placeholderFlag xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:arto="http://schemas.microsoft.com/office/word/2006/arto" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns="" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:w16sdtfl="http://schemas.microsoft.com/office/word/2024/wordml/sdtformatlock" xmlns:w16sdtdh="http://schemas.microsoft.com/office/word/2020/wordml/sdtdatahash" xmlns:w16du="http://schemas.microsoft.com/office/word/2023/wordml/word16du" xmlns:w16="http://schemas.microsoft.com/office/word/2018/wordml" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:w16cex="http://schemas.microsoft.com/office/word/2018/wordml/cex" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:oel="http://schemas.microsoft.com/office/2019/extlst" xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx8="http://schemas.microsoft.com/office/drawing/2016/5/14/chartex" xmlns:cx7="http://schemas.microsoft.com/office/drawing/2016/5/13/chartex" xmlns:cx6="http://schemas.microsoft.com/office/drawing/2016/5/12/chartex" xmlns:cx5="http://schemas.microsoft.com/office/drawing/2016/5/11/chartex" xmlns:cx4="http://schemas.microsoft.com/office/drawing/2016/5/10/chartex" xmlns:cx3="http://schemas.microsoft.com/office/drawing/2016/5/9/chartex" xmlns:cx2="http://schemas.microsoft.com/office/drawing/2015/10/21/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -2911,7 +2933,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2933,74 +2955,72 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B11" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
@@ -3032,8 +3052,8 @@
   </sheetPr>
   <dimension ref="A1:XFB1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29:O29"/>
+    <sheetView tabSelected="1" topLeftCell="H8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3061,15 +3081,15 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D3" s="5"/>
@@ -3106,47 +3126,47 @@
       <c r="E5" s="8"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
     </row>
     <row r="6" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
     </row>
     <row r="7" spans="3:16" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D8" s="5"/>
@@ -3194,13 +3214,13 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="K12" s="28" t="s">
-        <v>20</v>
+      <c r="K12" s="21" t="s">
+        <v>14</v>
       </c>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
     </row>
     <row r="13" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="5"/>
@@ -3216,7 +3236,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="K14" s="27" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
@@ -3237,7 +3257,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="K16" s="27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="L16" s="27"/>
       <c r="M16" s="27"/>
@@ -3249,7 +3269,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G17" s="5"/>
       <c r="K17" s="27"/>
@@ -3264,13 +3284,13 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="K18" s="34" t="s">
-        <v>24</v>
+      <c r="K18" s="28" t="s">
+        <v>18</v>
       </c>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
     </row>
     <row r="19" spans="3:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="5"/>
@@ -3285,11 +3305,11 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
     </row>
     <row r="21" spans="3:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C21" s="5"/>
@@ -3297,14 +3317,14 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="K21" s="29" t="str">
+      <c r="K21" s="25" t="str">
         <f>UPPER(student_name)</f>
-        <v>LORD JAISSON C. RIBERAL</v>
+        <v>CLIFF JASON D. DEYPALUBOS</v>
       </c>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
     </row>
     <row r="22" spans="3:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="5"/>
@@ -3312,11 +3332,11 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
     </row>
     <row r="23" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="5"/>
@@ -3324,7 +3344,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="K23" s="30" t="str">
+      <c r="K23" s="24" t="str" cm="1">
         <f t="array" ref="K23">_xlfn.LET(
  _xlpm.s,LOWER(TRIM(status)),
  _xlpm.prog,program,
@@ -3352,207 +3372,207 @@
  _xlpm.yos_txt,SUBSTITUTE(_xlpm.yos_raw,"-"," to "),
  _xlfn.SWITCH(TRUE(),
    OR(_xlpm.s="current student",_xlpm.s="current"),
-     "is a student currently enrolled in the "&amp;_xlpm.prog&amp;" program from "&amp;_xlpm.adm_year&amp;" to present.",
+     "is a student in this University currently enrolled in the "&amp;_xlpm.prog&amp;" program from "&amp;_xlpm.adm_year&amp;" to present.",
    OR(_xlpm.s="former student",_xlpm.s="former"),
-     "was a student enrolled in the "&amp;_xlpm.prog&amp;" program from "&amp;_xlpm.yos_txt&amp;".",
+     "was a student in this University enrolled in the "&amp;_xlpm.prog&amp;" program from "&amp;_xlpm.yos_txt&amp;".",
    OR(_xlpm.s="graduate",_xlpm.s="graduated",_xlpm.s="alumni",_xlpm.s="alum",_xlpm.s="alumni/graduate"),
-     "was enrolled in the "&amp;_xlpm.prog&amp;" program and has graduated"&amp;IF(_xlpm.grad_txt="",""," "&amp;_xlpm.grad_txt)&amp;".",
+     "is a Graduate in this University the "&amp;_xlpm.prog&amp;" program and has graduated"&amp;IF(_xlpm.grad_txt="",""," "&amp;_xlpm.grad_txt)&amp;".",
    ""
  )
 )</f>
-        <v>is a student currently enrolled in the Bachelor of Engineering Technology Major in Computer Engineering Technology program from 2022 to present.</v>
+        <v>was a student in this University enrolled in the Civil Engineering Technology program from 2015 to 2016.</v>
       </c>
-      <c r="L23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="30"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
     </row>
     <row r="24" spans="3:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
     </row>
     <row r="25" spans="3:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
     </row>
     <row r="26" spans="3:15" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="K26" s="30" t="str">
-        <f t="array" ref="K26">IF(LOWER(sex)="male","He",
+      <c r="K26" s="24" t="str">
+        <f>IF(LOWER(sex)="male","He",
    IF(LOWER(sex)="female","She","They")
  ) &amp;
  " " &amp;
  IF(status="Current Student","is","was") &amp;
- " of good moral character, with no record of violating university rules and regulations, and has not been subjected to any disciplinary action during " &amp;
+ " a student of good moral standing, has no records of violating the school rules and regulations, and has not been subjected to any disciplinary action during " &amp;
  IF(LOWER(sex)="male","his",IF(LOWER(sex)="female","her","their")) &amp;
- " stay."</f>
-        <v>She is of good moral character, with no record of violating university rules and regulations, and has not been subjected to any disciplinary action during her stay.</v>
+ " stay in the University."</f>
+        <v>He was a student of good moral standing, has no records of violating the school rules and regulations, and has not been subjected to any disciplinary action during his stay in the University.</v>
       </c>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
     </row>
     <row r="27" spans="3:15" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="K27" s="30" t="str">
+      <c r="K27" s="24" t="str">
         <f ca="1">_xlfn.LET(_xlpm.d,DAY(TODAY()),
      _xlpm.suf,IF(OR(_xlpm.d=11,_xlpm.d=12,_xlpm.d=13),"th",
             CHOOSE(1+MOD(_xlpm.d,10),"th","st","nd","rd","th","th","th","th","th","th")),
  "Given this " &amp; _xlpm.d &amp; _xlpm.suf &amp; " day of " &amp; TEXT(TODAY(),"mmmm yyyy") &amp;
  " at TUP Cavite Campus as a requirement for " &amp; purpose &amp; ".")</f>
-        <v>Given this 14th day of August 2025 at TUP Cavite Campus as a requirement for Scholarship.</v>
+        <v>Given this 18th day of August 2025 at TUP Cavite Campus as a requirement for continuing education.</v>
       </c>
-      <c r="L27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
-      <c r="O27" s="30"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
     </row>
     <row r="28" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
     </row>
     <row r="29" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
     </row>
     <row r="30" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
     </row>
     <row r="31" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
     </row>
     <row r="32" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
     </row>
     <row r="33" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
     </row>
     <row r="34" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
     </row>
     <row r="35" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
-      <c r="K35" s="32" t="str">
+      <c r="K35" s="23" t="str">
         <f t="array" ref="K35">UPPER(osahead)</f>
         <v>BEVERLY M. DE VEGA</v>
       </c>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="32"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
     </row>
     <row r="36" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
-      <c r="K36" s="31" t="s">
-        <v>25</v>
+      <c r="K36" s="22" t="s">
+        <v>19</v>
       </c>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="31"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
     </row>
     <row r="37" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
-      <c r="N37" s="28"/>
-      <c r="O37" s="28"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
     </row>
     <row r="38" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="28"/>
-      <c r="N38" s="28"/>
-      <c r="O38" s="28"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
     </row>
     <row r="39" spans="4:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D39" s="5"/>
@@ -3571,7 +3591,7 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="20" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -3584,66 +3604,66 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="28"/>
-      <c r="N41" s="28"/>
-      <c r="O41" s="28"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
     </row>
     <row r="42" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="28"/>
-      <c r="O42" s="28"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
     </row>
     <row r="43" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
-      <c r="K43" s="28"/>
-      <c r="L43" s="28"/>
-      <c r="M43" s="28"/>
-      <c r="N43" s="28"/>
-      <c r="O43" s="28"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
     </row>
     <row r="44" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="28"/>
-      <c r="N44" s="28"/>
-      <c r="O44" s="28"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="21"/>
     </row>
     <row r="45" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
-      <c r="K45" s="28"/>
-      <c r="L45" s="28"/>
-      <c r="M45" s="28"/>
-      <c r="N45" s="28"/>
-      <c r="O45" s="28"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="21"/>
     </row>
     <row r="46" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="28"/>
-      <c r="N46" s="28"/>
-      <c r="O46" s="28"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="21"/>
     </row>
     <row r="47" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D47" s="5"/>
@@ -9398,6 +9418,33 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="H2:P2"/>
+    <mergeCell ref="H5:P5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:P6"/>
+    <mergeCell ref="H7:P7"/>
+    <mergeCell ref="H9:P9"/>
+    <mergeCell ref="K16:O16"/>
+    <mergeCell ref="K17:O17"/>
+    <mergeCell ref="K18:O18"/>
+    <mergeCell ref="K20:O20"/>
+    <mergeCell ref="K12:O12"/>
+    <mergeCell ref="K14:O14"/>
+    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="K23:O24"/>
+    <mergeCell ref="K25:O25"/>
+    <mergeCell ref="K26:O26"/>
+    <mergeCell ref="K27:O27"/>
+    <mergeCell ref="K28:O28"/>
+    <mergeCell ref="K29:O29"/>
+    <mergeCell ref="K30:O30"/>
+    <mergeCell ref="K31:O31"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="K33:O33"/>
+    <mergeCell ref="K34:O34"/>
+    <mergeCell ref="K35:O35"/>
+    <mergeCell ref="K43:O43"/>
     <mergeCell ref="K44:O44"/>
     <mergeCell ref="K45:O45"/>
     <mergeCell ref="K46:O46"/>
@@ -9406,33 +9453,6 @@
     <mergeCell ref="K38:O38"/>
     <mergeCell ref="K41:O41"/>
     <mergeCell ref="K42:O42"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="K33:O33"/>
-    <mergeCell ref="K34:O34"/>
-    <mergeCell ref="K35:O35"/>
-    <mergeCell ref="K43:O43"/>
-    <mergeCell ref="K27:O27"/>
-    <mergeCell ref="K28:O28"/>
-    <mergeCell ref="K29:O29"/>
-    <mergeCell ref="K30:O30"/>
-    <mergeCell ref="K31:O31"/>
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="K22:O22"/>
-    <mergeCell ref="K23:O24"/>
-    <mergeCell ref="K25:O25"/>
-    <mergeCell ref="K26:O26"/>
-    <mergeCell ref="H9:P9"/>
-    <mergeCell ref="K16:O16"/>
-    <mergeCell ref="K17:O17"/>
-    <mergeCell ref="K18:O18"/>
-    <mergeCell ref="K20:O20"/>
-    <mergeCell ref="K12:O12"/>
-    <mergeCell ref="K14:O14"/>
-    <mergeCell ref="H2:P2"/>
-    <mergeCell ref="H5:P5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:P6"/>
-    <mergeCell ref="H7:P7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D6" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -9441,7 +9461,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.55972222222222201" right="0.2" top="0.2" bottom="0.2" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="95" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="7" max="1048575" man="1"/>
   </colBreaks>
@@ -10465,239 +10485,239 @@
   <sheetData>
     <row r="2" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="12:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="L9" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="S19" s="3"/>
+    </row>
+    <row r="20" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S21" s="6"/>
+    </row>
+    <row r="22" spans="11:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="34" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L3" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L4" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L5" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L6" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L7" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" spans="12:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="L9" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="11:19" x14ac:dyDescent="0.25">
-      <c r="S19" s="3"/>
-    </row>
-    <row r="20" spans="11:19" x14ac:dyDescent="0.25">
-      <c r="S20" s="6"/>
-    </row>
-    <row r="21" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S21" s="6"/>
-    </row>
-    <row r="22" spans="11:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K22" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
       <c r="S22" s="9"/>
     </row>
     <row r="23" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
       <c r="S23" s="9"/>
     </row>
     <row r="24" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
       <c r="S24" s="10"/>
     </row>
     <row r="25" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
       <c r="S25" s="11"/>
     </row>
     <row r="26" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="34"/>
       <c r="S26" s="16"/>
     </row>
     <row r="27" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="34"/>
     </row>
     <row r="28" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="34"/>
     </row>
     <row r="29" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
     </row>
     <row r="30" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34"/>
     </row>
     <row r="31" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="34"/>
     </row>
     <row r="32" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="33"/>
-      <c r="O32" s="33"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="34"/>
+      <c r="O32" s="34"/>
     </row>
     <row r="33" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="33"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
+      <c r="O33" s="34"/>
     </row>
     <row r="34" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
-      <c r="N34" s="33"/>
-      <c r="O34" s="33"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="34"/>
     </row>
     <row r="35" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K35" s="33"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="33"/>
-      <c r="O35" s="33"/>
+      <c r="K35" s="34"/>
+      <c r="L35" s="34"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="34"/>
+      <c r="O35" s="34"/>
     </row>
     <row r="36" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K36" s="33"/>
-      <c r="L36" s="33"/>
-      <c r="M36" s="33"/>
-      <c r="N36" s="33"/>
-      <c r="O36" s="33"/>
+      <c r="K36" s="34"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="34"/>
+      <c r="O36" s="34"/>
     </row>
     <row r="37" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="33"/>
-      <c r="N37" s="33"/>
-      <c r="O37" s="33"/>
+      <c r="K37" s="34"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="34"/>
+      <c r="O37" s="34"/>
     </row>
     <row r="38" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K38" s="33"/>
-      <c r="L38" s="33"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="33"/>
-      <c r="O38" s="33"/>
+      <c r="K38" s="34"/>
+      <c r="L38" s="34"/>
+      <c r="M38" s="34"/>
+      <c r="N38" s="34"/>
+      <c r="O38" s="34"/>
     </row>
     <row r="39" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K39" s="33"/>
-      <c r="L39" s="33"/>
-      <c r="M39" s="33"/>
-      <c r="N39" s="33"/>
-      <c r="O39" s="33"/>
+      <c r="K39" s="34"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
     </row>
     <row r="40" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
+      <c r="K40" s="34"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="34"/>
+      <c r="N40" s="34"/>
+      <c r="O40" s="34"/>
     </row>
     <row r="41" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
+      <c r="K41" s="34"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="34"/>
+      <c r="N41" s="34"/>
+      <c r="O41" s="34"/>
     </row>
     <row r="42" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K42" s="33"/>
-      <c r="L42" s="33"/>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
-      <c r="O42" s="33"/>
+      <c r="K42" s="34"/>
+      <c r="L42" s="34"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
+      <c r="O42" s="34"/>
     </row>
     <row r="43" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K43" s="33"/>
-      <c r="L43" s="33"/>
-      <c r="M43" s="33"/>
-      <c r="N43" s="33"/>
-      <c r="O43" s="33"/>
+      <c r="K43" s="34"/>
+      <c r="L43" s="34"/>
+      <c r="M43" s="34"/>
+      <c r="N43" s="34"/>
+      <c r="O43" s="34"/>
     </row>
     <row r="44" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K44" s="33"/>
-      <c r="L44" s="33"/>
-      <c r="M44" s="33"/>
-      <c r="N44" s="33"/>
-      <c r="O44" s="33"/>
+      <c r="K44" s="34"/>
+      <c r="L44" s="34"/>
+      <c r="M44" s="34"/>
+      <c r="N44" s="34"/>
+      <c r="O44" s="34"/>
     </row>
     <row r="45" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K45" s="33"/>
-      <c r="L45" s="33"/>
-      <c r="M45" s="33"/>
-      <c r="N45" s="33"/>
-      <c r="O45" s="33"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="34"/>
+      <c r="M45" s="34"/>
+      <c r="N45" s="34"/>
+      <c r="O45" s="34"/>
     </row>
     <row r="46" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K46" s="33"/>
-      <c r="L46" s="33"/>
-      <c r="M46" s="33"/>
-      <c r="N46" s="33"/>
-      <c r="O46" s="33"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="34"/>
+      <c r="M46" s="34"/>
+      <c r="N46" s="34"/>
+      <c r="O46" s="34"/>
     </row>
     <row r="47" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K47" s="33"/>
-      <c r="L47" s="33"/>
-      <c r="M47" s="33"/>
-      <c r="N47" s="33"/>
-      <c r="O47" s="33"/>
+      <c r="K47" s="34"/>
+      <c r="L47" s="34"/>
+      <c r="M47" s="34"/>
+      <c r="N47" s="34"/>
+      <c r="O47" s="34"/>
     </row>
     <row r="48" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
latest update = libre bugs
</commit_message>
<xml_diff>
--- a/myapp/cert_templates/good-moral-form.xlsx
+++ b/myapp/cert_templates/good-moral-form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\thesis_osa\myproject\myapp\cert_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA53A22-79A8-40D0-BFD4-29C1C1DA7CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDFC6FF-CF7D-4DE5-BF64-F43A167788BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,28 +51,6 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </valueMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
@@ -83,9 +61,6 @@
   </si>
   <si>
     <t>student_name</t>
-  </si>
-  <si>
-    <t>LORD JAISSON C. RIBERAL N/A</t>
   </si>
   <si>
     <t>program</t>
@@ -154,9 +129,6 @@
     <t>Head, Office of Student Affairs</t>
   </si>
   <si>
-    <t xml:space="preserve">   PC-F-OQA-DCG-14 Ø3 (03.28.25)</t>
-  </si>
-  <si>
     <t>REPUBLIC OF THE PHILIPPINES</t>
   </si>
   <si>
@@ -185,6 +157,12 @@
 and has not been subjected to any disciplinary action 
 during her stay in the University.
 Given this 13th day of June 2022 at TUP Cavite Campus for enrollment purposes.</t>
+  </si>
+  <si>
+    <t>LORD JAISSON C. RIBERAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      PC-F-OQA-DCG-14 Ø3 (03.28.25)</t>
   </si>
 </sst>
 </file>
@@ -355,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -410,6 +388,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -633,15 +614,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>68721</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>148774</xdr:rowOff>
+      <xdr:colOff>152146</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>27248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>13138</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>79935</xdr:rowOff>
+      <xdr:colOff>96563</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>53002</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -671,8 +652,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="68721" y="1396877"/>
-          <a:ext cx="2394641" cy="8575920"/>
+          <a:off x="152146" y="1522673"/>
+          <a:ext cx="2401867" cy="8626829"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1852,65 +1833,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <fb t="e">#NAME?</fb>
-    <v>4</v>
-    <v>1</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_error">
-    <k n="errorType" t="i"/>
-    <k n="subType" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -2090,7 +2012,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2112,72 +2034,72 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
@@ -2207,10 +2129,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:XFB1002"/>
+  <dimension ref="A1:XFB1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12:O12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32:O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2238,15 +2160,15 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D3" s="5"/>
@@ -2283,47 +2205,47 @@
       <c r="E5" s="10"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
     </row>
     <row r="6" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
     </row>
     <row r="7" spans="3:16" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D8" s="5"/>
@@ -2338,179 +2260,187 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-    </row>
-    <row r="10" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+    </row>
+    <row r="10" spans="3:16" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="5"/>
       <c r="D10" s="12"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="3:16" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+    </row>
+    <row r="11" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="5"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="5" t="b">
-        <f>IF(D10="Not Graduate",_xlfn.CONCAT("from ",VLOOKUP($D$6,#REF!,4,FALSE())," to present."))</f>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="3:16" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="5"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="5" t="b">
+        <f>IF(D11="Not Graduate",_xlfn.CONCAT("from ",VLOOKUP($D$6,#REF!,4,FALSE())," to present."))</f>
         <v>0</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="3:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="5"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="K12" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-    </row>
-    <row r="13" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="3:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="5"/>
-      <c r="D13" s="12"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="3:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="K13" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+    </row>
+    <row r="14" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="5"/>
       <c r="D14" s="12"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="K14" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-    </row>
-    <row r="15" spans="3:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="3:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C15" s="5"/>
       <c r="D15" s="12"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="3:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="K15" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+    </row>
+    <row r="16" spans="3:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
       <c r="D16" s="12"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="K16" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-    </row>
-    <row r="17" spans="3:15" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="3:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C17" s="5"/>
       <c r="D17" s="12"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
-        <v>23</v>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="K17" s="29" t="s">
+        <v>21</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-    </row>
-    <row r="18" spans="3:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+    </row>
+    <row r="18" spans="3:15" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C18" s="5"/>
       <c r="D18" s="12"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="G18" s="5"/>
-      <c r="K18" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-    </row>
-    <row r="19" spans="3:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+    </row>
+    <row r="19" spans="3:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="3:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+    </row>
+    <row r="20" spans="3:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-    </row>
-    <row r="21" spans="3:15" ht="26.25" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="3:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="K21" s="26" t="e" vm="1">
-        <f ca="1">UPPER(
-  TRIM(
-    _xlfn.ORG.LIBREOFFICE.REGEX(
-      student_name,
-      "(?:\s*[\(\[]?\s*(?i)(?:N/?A|NONE)\s*[\)\]]?\s*)+$",
-      ""
-    )
-  )
-)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-    </row>
-    <row r="22" spans="3:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+    </row>
+    <row r="22" spans="3:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-    </row>
-    <row r="23" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="27" t="str">
+        <f>UPPER(student_name)</f>
+        <v>LORD JAISSON C. RIBERAL</v>
+      </c>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+    </row>
+    <row r="23" spans="3:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="K23" s="24" t="str">
-        <f t="array" ref="K23">_xlfn.LET(
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+    </row>
+    <row r="24" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="K24" s="25" t="str">
+        <f t="array" ref="K24">_xlfn.LET(
  _xlpm.s,LOWER(TRIM(status)),
  _xlpm.prog,program,
  _xlpm.adm_raw,admission_date,
@@ -2547,39 +2477,39 @@
 )</f>
         <v>was a student in this University enrolled in the Civil Engineering Technology program from 2015 to 2016.</v>
       </c>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-    </row>
-    <row r="24" spans="3:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-    </row>
-    <row r="25" spans="3:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+    </row>
+    <row r="25" spans="3:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-    </row>
-    <row r="26" spans="3:15" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+    </row>
+    <row r="26" spans="3:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="K26" s="24" t="str">
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+    </row>
+    <row r="27" spans="3:15" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="K27" s="25" t="str">
         <f>IF(LOWER(sex)="male","He",
    IF(LOWER(sex)="female","She","They")
  ) &amp;
@@ -2590,17 +2520,17 @@
  " stay in the University."</f>
         <v>He was a student of good moral standing, has no records of violating the school rules and regulations, and has not been subjected to any disciplinary action during his stay in the University.</v>
       </c>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-    </row>
-    <row r="27" spans="3:15" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="K27" s="24" t="str">
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+    </row>
+    <row r="28" spans="3:15" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="K28" s="25" t="str">
         <f ca="1">_xlfn.LET(_xlpm.d,DAY(TODAY()),
      _xlpm.suf,IF(OR(_xlpm.d=11,_xlpm.d=12,_xlpm.d=13),"th",
             CHOOSE(1+MOD(_xlpm.d,10),"th","st","nd","rd","th","th","th","th","th","th")),
@@ -2608,238 +2538,227 @@
  " at TUP Cavite Campus as a requirement for " &amp; purpose &amp; ".")</f>
         <v>Given this 24th day of August 2025 at TUP Cavite Campus as a requirement for continuing education.</v>
       </c>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-    </row>
-    <row r="28" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
     </row>
     <row r="29" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
     </row>
     <row r="30" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
     </row>
     <row r="31" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
     </row>
     <row r="32" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
     </row>
     <row r="33" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
     </row>
     <row r="34" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="24"/>
     </row>
     <row r="35" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
-      <c r="K35" s="22" t="str">
-        <f t="array" ref="K35">UPPER(osahead)</f>
-        <v>BEVERLY M. DE VEGA</v>
-      </c>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="24"/>
     </row>
     <row r="36" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
-      <c r="K36" s="23" t="s">
-        <v>25</v>
+      <c r="K36" s="23" t="str">
+        <f t="array" ref="K36">UPPER(osahead)</f>
+        <v>BEVERLY M. DE VEGA</v>
       </c>
       <c r="L36" s="23"/>
       <c r="M36" s="23"/>
       <c r="N36" s="23"/>
       <c r="O36" s="23"/>
     </row>
-    <row r="37" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
-      <c r="N37" s="21"/>
-      <c r="O37" s="21"/>
+      <c r="K37" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
     </row>
     <row r="38" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="21"/>
-      <c r="N38" s="21"/>
-      <c r="O38" s="21"/>
-    </row>
-    <row r="39" spans="4:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+    </row>
+    <row r="39" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-    </row>
-    <row r="40" spans="4:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="22"/>
+      <c r="O39" s="22"/>
+    </row>
+    <row r="40" spans="4:15" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
-      <c r="H40" s="14" t="s">
-        <v>26</v>
-      </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
     </row>
-    <row r="41" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
-      <c r="O41" s="21"/>
-    </row>
-    <row r="42" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+    </row>
+    <row r="42" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-      <c r="K42" s="21"/>
-      <c r="L42" s="21"/>
-      <c r="M42" s="21"/>
-      <c r="N42" s="21"/>
-      <c r="O42" s="21"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="22"/>
+      <c r="N42" s="22"/>
+      <c r="O42" s="22"/>
     </row>
     <row r="43" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="21"/>
-      <c r="M43" s="21"/>
-      <c r="N43" s="21"/>
-      <c r="O43" s="21"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
+      <c r="M43" s="22"/>
+      <c r="N43" s="22"/>
+      <c r="O43" s="22"/>
     </row>
     <row r="44" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
-      <c r="K44" s="21"/>
-      <c r="L44" s="21"/>
-      <c r="M44" s="21"/>
-      <c r="N44" s="21"/>
-      <c r="O44" s="21"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="22"/>
+      <c r="O44" s="22"/>
     </row>
     <row r="45" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
-      <c r="K45" s="21"/>
-      <c r="L45" s="21"/>
-      <c r="M45" s="21"/>
-      <c r="N45" s="21"/>
-      <c r="O45" s="21"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="22"/>
+      <c r="M45" s="22"/>
+      <c r="N45" s="22"/>
+      <c r="O45" s="22"/>
     </row>
     <row r="46" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
-      <c r="K46" s="21"/>
-      <c r="L46" s="21"/>
-      <c r="M46" s="21"/>
-      <c r="N46" s="21"/>
-      <c r="O46" s="21"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="22"/>
+      <c r="N46" s="22"/>
+      <c r="O46" s="22"/>
     </row>
     <row r="47" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="22"/>
+      <c r="N47" s="22"/>
+      <c r="O47" s="22"/>
     </row>
     <row r="48" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D48" s="5"/>
@@ -2868,6 +2787,11 @@
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="15"/>
     </row>
     <row r="51" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D51" s="5"/>
@@ -8580,6 +8504,12 @@
       <c r="E1002" s="5"/>
       <c r="F1002" s="5"/>
       <c r="G1002" s="5"/>
+    </row>
+    <row r="1003" spans="4:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1003" s="5"/>
+      <c r="E1003" s="5"/>
+      <c r="F1003" s="5"/>
+      <c r="G1003" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="35">
@@ -8589,16 +8519,15 @@
     <mergeCell ref="H6:P6"/>
     <mergeCell ref="H7:P7"/>
     <mergeCell ref="H9:P9"/>
-    <mergeCell ref="K12:O12"/>
-    <mergeCell ref="K14:O14"/>
-    <mergeCell ref="K16:O16"/>
+    <mergeCell ref="K13:O13"/>
+    <mergeCell ref="K15:O15"/>
     <mergeCell ref="K17:O17"/>
     <mergeCell ref="K18:O18"/>
-    <mergeCell ref="K20:O20"/>
+    <mergeCell ref="K19:O19"/>
     <mergeCell ref="K21:O21"/>
     <mergeCell ref="K22:O22"/>
-    <mergeCell ref="K23:O24"/>
-    <mergeCell ref="K25:O25"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="K24:O25"/>
     <mergeCell ref="K26:O26"/>
     <mergeCell ref="K27:O27"/>
     <mergeCell ref="K28:O28"/>
@@ -8612,12 +8541,13 @@
     <mergeCell ref="K36:O36"/>
     <mergeCell ref="K37:O37"/>
     <mergeCell ref="K38:O38"/>
-    <mergeCell ref="K41:O41"/>
+    <mergeCell ref="K39:O39"/>
     <mergeCell ref="K42:O42"/>
     <mergeCell ref="K43:O43"/>
     <mergeCell ref="K44:O44"/>
     <mergeCell ref="K45:O45"/>
     <mergeCell ref="K46:O46"/>
+    <mergeCell ref="K47:O47"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D6" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -9650,239 +9580,239 @@
   <sheetData>
     <row r="2" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L3" s="16" t="s">
+    <row r="5" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L4" s="16" t="s">
+    <row r="6" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L5" s="17" t="s">
+    <row r="7" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L6" s="17" t="s">
+    <row r="8" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="12:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="L9" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="S19" s="3"/>
+    </row>
+    <row r="20" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="S20" s="16"/>
+    </row>
+    <row r="21" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S21" s="16"/>
+    </row>
+    <row r="22" spans="11:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="34" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L7" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" spans="12:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="L9" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="11:19" x14ac:dyDescent="0.25">
-      <c r="S19" s="3"/>
-    </row>
-    <row r="20" spans="11:19" x14ac:dyDescent="0.25">
-      <c r="S20" s="16"/>
-    </row>
-    <row r="21" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S21" s="16"/>
-    </row>
-    <row r="22" spans="11:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K22" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
       <c r="S22" s="17"/>
     </row>
     <row r="23" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
       <c r="S23" s="17"/>
     </row>
     <row r="24" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
       <c r="S24" s="20"/>
     </row>
     <row r="25" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
       <c r="S25" s="11"/>
     </row>
     <row r="26" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="34"/>
       <c r="S26" s="19"/>
     </row>
     <row r="27" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="34"/>
     </row>
     <row r="28" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="34"/>
     </row>
     <row r="29" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
     </row>
     <row r="30" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34"/>
     </row>
     <row r="31" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="34"/>
     </row>
     <row r="32" spans="11:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="33"/>
-      <c r="O32" s="33"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="34"/>
+      <c r="O32" s="34"/>
     </row>
     <row r="33" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="33"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
+      <c r="O33" s="34"/>
     </row>
     <row r="34" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
-      <c r="N34" s="33"/>
-      <c r="O34" s="33"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="34"/>
     </row>
     <row r="35" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K35" s="33"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="33"/>
-      <c r="O35" s="33"/>
+      <c r="K35" s="34"/>
+      <c r="L35" s="34"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="34"/>
+      <c r="O35" s="34"/>
     </row>
     <row r="36" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K36" s="33"/>
-      <c r="L36" s="33"/>
-      <c r="M36" s="33"/>
-      <c r="N36" s="33"/>
-      <c r="O36" s="33"/>
+      <c r="K36" s="34"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="34"/>
+      <c r="O36" s="34"/>
     </row>
     <row r="37" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="33"/>
-      <c r="N37" s="33"/>
-      <c r="O37" s="33"/>
+      <c r="K37" s="34"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="34"/>
+      <c r="O37" s="34"/>
     </row>
     <row r="38" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K38" s="33"/>
-      <c r="L38" s="33"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="33"/>
-      <c r="O38" s="33"/>
+      <c r="K38" s="34"/>
+      <c r="L38" s="34"/>
+      <c r="M38" s="34"/>
+      <c r="N38" s="34"/>
+      <c r="O38" s="34"/>
     </row>
     <row r="39" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K39" s="33"/>
-      <c r="L39" s="33"/>
-      <c r="M39" s="33"/>
-      <c r="N39" s="33"/>
-      <c r="O39" s="33"/>
+      <c r="K39" s="34"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
     </row>
     <row r="40" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
+      <c r="K40" s="34"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="34"/>
+      <c r="N40" s="34"/>
+      <c r="O40" s="34"/>
     </row>
     <row r="41" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
+      <c r="K41" s="34"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="34"/>
+      <c r="N41" s="34"/>
+      <c r="O41" s="34"/>
     </row>
     <row r="42" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K42" s="33"/>
-      <c r="L42" s="33"/>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
-      <c r="O42" s="33"/>
+      <c r="K42" s="34"/>
+      <c r="L42" s="34"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
+      <c r="O42" s="34"/>
     </row>
     <row r="43" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K43" s="33"/>
-      <c r="L43" s="33"/>
-      <c r="M43" s="33"/>
-      <c r="N43" s="33"/>
-      <c r="O43" s="33"/>
+      <c r="K43" s="34"/>
+      <c r="L43" s="34"/>
+      <c r="M43" s="34"/>
+      <c r="N43" s="34"/>
+      <c r="O43" s="34"/>
     </row>
     <row r="44" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K44" s="33"/>
-      <c r="L44" s="33"/>
-      <c r="M44" s="33"/>
-      <c r="N44" s="33"/>
-      <c r="O44" s="33"/>
+      <c r="K44" s="34"/>
+      <c r="L44" s="34"/>
+      <c r="M44" s="34"/>
+      <c r="N44" s="34"/>
+      <c r="O44" s="34"/>
     </row>
     <row r="45" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K45" s="33"/>
-      <c r="L45" s="33"/>
-      <c r="M45" s="33"/>
-      <c r="N45" s="33"/>
-      <c r="O45" s="33"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="34"/>
+      <c r="M45" s="34"/>
+      <c r="N45" s="34"/>
+      <c r="O45" s="34"/>
     </row>
     <row r="46" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K46" s="33"/>
-      <c r="L46" s="33"/>
-      <c r="M46" s="33"/>
-      <c r="N46" s="33"/>
-      <c r="O46" s="33"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="34"/>
+      <c r="M46" s="34"/>
+      <c r="N46" s="34"/>
+      <c r="O46" s="34"/>
     </row>
     <row r="47" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K47" s="33"/>
-      <c r="L47" s="33"/>
-      <c r="M47" s="33"/>
-      <c r="N47" s="33"/>
-      <c r="O47" s="33"/>
+      <c r="K47" s="34"/>
+      <c r="L47" s="34"/>
+      <c r="M47" s="34"/>
+      <c r="N47" s="34"/>
+      <c r="O47" s="34"/>
     </row>
     <row r="48" spans="11:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ADJUST GOOD MORAL FORM
</commit_message>
<xml_diff>
--- a/myapp/cert_templates/good-moral-form.xlsx
+++ b/myapp/cert_templates/good-moral-form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\thesis_osa\myproject\myapp\cert_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDFC6FF-CF7D-4DE5-BF64-F43A167788BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C4C59F-A35F-4DB0-BA6C-D2D73BDE49B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="student_name">inputs!$B$2</definedName>
     <definedName name="years_of_stay">inputs!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -333,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -393,30 +393,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -428,8 +404,35 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2132,7 +2135,7 @@
   <dimension ref="A1:XFB1003"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32:O32"/>
+      <selection activeCell="K33" sqref="K33:O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2160,15 +2163,15 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D3" s="5"/>
@@ -2205,30 +2208,30 @@
       <c r="E5" s="10"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
     </row>
     <row r="6" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
     </row>
     <row r="7" spans="3:16" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="5" t="s">
@@ -2237,15 +2240,15 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D8" s="5"/>
@@ -2260,15 +2263,15 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
     </row>
     <row r="10" spans="3:16" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="5"/>
@@ -2309,13 +2312,13 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="K13" s="22" t="s">
+      <c r="K13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
     </row>
     <row r="14" spans="3:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="5"/>
@@ -2330,13 +2333,13 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="K15" s="29" t="s">
+      <c r="K15" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
     </row>
     <row r="16" spans="3:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
@@ -2351,13 +2354,13 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
     </row>
     <row r="18" spans="3:15" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C18" s="5"/>
@@ -2367,11 +2370,11 @@
         <v>22</v>
       </c>
       <c r="G18" s="5"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
     </row>
     <row r="19" spans="3:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="5"/>
@@ -2379,13 +2382,13 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="K19" s="26" t="s">
+      <c r="K19" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
     </row>
     <row r="20" spans="3:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="5"/>
@@ -2400,11 +2403,11 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
     </row>
     <row r="22" spans="3:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C22" s="5"/>
@@ -2412,14 +2415,14 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="K22" s="27" t="str">
+      <c r="K22" s="30" t="str">
         <f>UPPER(student_name)</f>
         <v>LORD JAISSON C. RIBERAL</v>
       </c>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
     </row>
     <row r="23" spans="3:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="5"/>
@@ -2427,11 +2430,11 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
     </row>
     <row r="24" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="5"/>
@@ -2439,7 +2442,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="K24" s="25" t="str">
+      <c r="K24" s="31" t="str">
         <f t="array" ref="K24">_xlfn.LET(
  _xlpm.s,LOWER(TRIM(status)),
  _xlpm.prog,program,
@@ -2477,39 +2480,39 @@
 )</f>
         <v>was a student in this University enrolled in the Civil Engineering Technology program from 2015 to 2016.</v>
       </c>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
     </row>
     <row r="25" spans="3:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
     </row>
     <row r="26" spans="3:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
     </row>
     <row r="27" spans="3:15" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="K27" s="25" t="str">
+      <c r="K27" s="31" t="str">
         <f>IF(LOWER(sex)="male","He",
    IF(LOWER(sex)="female","She","They")
  ) &amp;
@@ -2520,165 +2523,165 @@
  " stay in the University."</f>
         <v>He was a student of good moral standing, has no records of violating the school rules and regulations, and has not been subjected to any disciplinary action during his stay in the University.</v>
       </c>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
     </row>
     <row r="28" spans="3:15" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="K28" s="25" t="str">
+      <c r="K28" s="31" t="str">
         <f ca="1">_xlfn.LET(_xlpm.d,DAY(TODAY()),
      _xlpm.suf,IF(OR(_xlpm.d=11,_xlpm.d=12,_xlpm.d=13),"th",
             CHOOSE(1+MOD(_xlpm.d,10),"th","st","nd","rd","th","th","th","th","th","th")),
  "Given this " &amp; _xlpm.d &amp; _xlpm.suf &amp; " day of " &amp; TEXT(TODAY(),"mmmm yyyy") &amp;
  " at TUP Cavite Campus as a requirement for " &amp; purpose &amp; ".")</f>
-        <v>Given this 24th day of August 2025 at TUP Cavite Campus as a requirement for continuing education.</v>
+        <v>Given this 27th day of August 2025 at TUP Cavite Campus as a requirement for continuing education.</v>
       </c>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
     </row>
     <row r="29" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
     </row>
     <row r="30" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
     </row>
     <row r="31" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
     </row>
     <row r="32" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="24"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
     </row>
     <row r="33" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="24"/>
-      <c r="O33" s="24"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
     </row>
     <row r="34" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="24"/>
-      <c r="O34" s="24"/>
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
     </row>
     <row r="35" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="24"/>
-      <c r="O35" s="24"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="32"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="32"/>
     </row>
     <row r="36" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
-      <c r="K36" s="23" t="str">
-        <f t="array" ref="K36">UPPER(osahead)</f>
-        <v>BEVERLY M. DE VEGA</v>
-      </c>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="23"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
     </row>
     <row r="37" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
-      <c r="K37" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="L37" s="24"/>
-      <c r="M37" s="24"/>
-      <c r="N37" s="24"/>
-      <c r="O37" s="24"/>
+      <c r="K37" s="32"/>
+      <c r="L37" s="32"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="32"/>
     </row>
     <row r="38" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
-      <c r="O38" s="22"/>
-    </row>
-    <row r="39" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="27"/>
+    </row>
+    <row r="39" spans="4:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="22"/>
+      <c r="K39" s="33" t="str">
+        <f t="array" ref="K39">UPPER(osahead)</f>
+        <v>BEVERLY M. DE VEGA</v>
+      </c>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
     </row>
     <row r="40" spans="4:15" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
+      <c r="K40" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
     </row>
     <row r="41" spans="4:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D41" s="5"/>
@@ -2699,66 +2702,66 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
+      <c r="N42" s="27"/>
+      <c r="O42" s="27"/>
     </row>
     <row r="43" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="22"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
+      <c r="N43" s="27"/>
+      <c r="O43" s="27"/>
     </row>
     <row r="44" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
+      <c r="N44" s="27"/>
+      <c r="O44" s="27"/>
     </row>
     <row r="45" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="22"/>
-      <c r="M45" s="22"/>
-      <c r="N45" s="22"/>
-      <c r="O45" s="22"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="27"/>
+      <c r="O45" s="27"/>
     </row>
     <row r="46" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="27"/>
+      <c r="N46" s="27"/>
+      <c r="O46" s="27"/>
     </row>
     <row r="47" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
-      <c r="K47" s="22"/>
-      <c r="L47" s="22"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="22"/>
-      <c r="O47" s="22"/>
+      <c r="K47" s="27"/>
+      <c r="L47" s="27"/>
+      <c r="M47" s="27"/>
+      <c r="N47" s="27"/>
+      <c r="O47" s="27"/>
     </row>
     <row r="48" spans="4:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D48" s="5"/>
@@ -8512,42 +8515,43 @@
       <c r="G1003" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="36">
+    <mergeCell ref="K43:O43"/>
+    <mergeCell ref="K44:O44"/>
+    <mergeCell ref="K45:O45"/>
+    <mergeCell ref="K46:O46"/>
+    <mergeCell ref="K47:O47"/>
+    <mergeCell ref="K36:O36"/>
+    <mergeCell ref="K37:O37"/>
+    <mergeCell ref="K38:O38"/>
+    <mergeCell ref="K39:O39"/>
+    <mergeCell ref="K42:O42"/>
+    <mergeCell ref="K40:O40"/>
+    <mergeCell ref="K31:O31"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="K33:O33"/>
+    <mergeCell ref="K34:O34"/>
+    <mergeCell ref="K35:O35"/>
+    <mergeCell ref="K26:O26"/>
+    <mergeCell ref="K27:O27"/>
+    <mergeCell ref="K28:O28"/>
+    <mergeCell ref="K29:O29"/>
+    <mergeCell ref="K30:O30"/>
+    <mergeCell ref="K19:O19"/>
+    <mergeCell ref="K21:O21"/>
+    <mergeCell ref="K22:O22"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="K24:O25"/>
+    <mergeCell ref="H9:P9"/>
+    <mergeCell ref="K13:O13"/>
+    <mergeCell ref="K15:O15"/>
+    <mergeCell ref="K17:O17"/>
+    <mergeCell ref="K18:O18"/>
     <mergeCell ref="H2:P2"/>
     <mergeCell ref="H5:P5"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="H6:P6"/>
     <mergeCell ref="H7:P7"/>
-    <mergeCell ref="H9:P9"/>
-    <mergeCell ref="K13:O13"/>
-    <mergeCell ref="K15:O15"/>
-    <mergeCell ref="K17:O17"/>
-    <mergeCell ref="K18:O18"/>
-    <mergeCell ref="K19:O19"/>
-    <mergeCell ref="K21:O21"/>
-    <mergeCell ref="K22:O22"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="K24:O25"/>
-    <mergeCell ref="K26:O26"/>
-    <mergeCell ref="K27:O27"/>
-    <mergeCell ref="K28:O28"/>
-    <mergeCell ref="K29:O29"/>
-    <mergeCell ref="K30:O30"/>
-    <mergeCell ref="K31:O31"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="K33:O33"/>
-    <mergeCell ref="K34:O34"/>
-    <mergeCell ref="K35:O35"/>
-    <mergeCell ref="K36:O36"/>
-    <mergeCell ref="K37:O37"/>
-    <mergeCell ref="K38:O38"/>
-    <mergeCell ref="K39:O39"/>
-    <mergeCell ref="K42:O42"/>
-    <mergeCell ref="K43:O43"/>
-    <mergeCell ref="K44:O44"/>
-    <mergeCell ref="K45:O45"/>
-    <mergeCell ref="K46:O46"/>
-    <mergeCell ref="K47:O47"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D6" xr:uid="{00000000-0002-0000-0100-000000000000}">

</xml_diff>